<commit_message>
Update Berekening capaciteit - hardheid - AQMOS Waterontharders.xlsx
</commit_message>
<xml_diff>
--- a/readme/manuals/Berekening capaciteit - hardheid - AQMOS Waterontharders.xlsx
+++ b/readme/manuals/Berekening capaciteit - hardheid - AQMOS Waterontharders.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Drive Aqmos\Documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fonske\Documents\GitHub\clack-reader-v4\readme\manuals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F74C61-9B2F-4BEA-BCFF-F0F1EDF604D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620D8B11-D3D6-4C8A-BCC5-82A6B59A1C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AAFCFBBE-F434-4872-BD78-77559D0951A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AAFCFBBE-F434-4872-BD78-77559D0951A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -20,15 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -600,6 +591,30 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -609,33 +624,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="7" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -748,7 +739,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1047,7 +1038,7 @@
   <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:H16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,17 +1057,17 @@
         <v>10</v>
       </c>
       <c r="C2" s="9"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="str">
         <f>B3</f>
-        <v>LESS-10</v>
+        <v>LESS-15</v>
       </c>
       <c r="L2" s="15">
         <v>-0.1</v>
@@ -1085,14 +1076,14 @@
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="17"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
       <c r="J3" s="2"/>
       <c r="K3" s="12" t="s">
         <v>5</v>
@@ -1100,7 +1091,7 @@
       <c r="L3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="42"/>
+      <c r="M3" s="36"/>
       <c r="N3" s="9" t="s">
         <v>22</v>
       </c>
@@ -1110,15 +1101,15 @@
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
       <c r="J4" s="3"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="43"/>
+      <c r="M4" s="37"/>
       <c r="N4" t="s">
         <v>2</v>
       </c>
@@ -1131,23 +1122,23 @@
         <f>IF($B$3="Anders", "Aantal liters hars:", "")</f>
         <v/>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
       <c r="J5" s="4">
         <v>7.5</v>
       </c>
       <c r="K5" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J5*0.17811)*Data!$F$2), 100)</f>
-        <v>3700</v>
+        <v>5600</v>
       </c>
       <c r="L5" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J5*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>3300</v>
-      </c>
-      <c r="M5" s="44"/>
+        <v>5000</v>
+      </c>
+      <c r="M5" s="38"/>
       <c r="N5" t="s">
         <v>3</v>
       </c>
@@ -1158,23 +1149,23 @@
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25"/>
       <c r="C6" s="17"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
       <c r="J6" s="5">
         <v>10</v>
       </c>
       <c r="K6" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J6*0.17811)*Data!$F$2), 100)</f>
-        <v>2800</v>
+        <v>4200</v>
       </c>
       <c r="L6" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J6*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>2500</v>
-      </c>
-      <c r="M6" s="44"/>
+        <v>3700</v>
+      </c>
+      <c r="M6" s="38"/>
       <c r="N6" t="s">
         <v>4</v>
       </c>
@@ -1184,21 +1175,21 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="16"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
       <c r="J7" s="6">
         <v>11</v>
       </c>
       <c r="K7" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J7*0.17811)*Data!$F$2), 100)</f>
-        <v>2500</v>
+        <v>3800</v>
       </c>
       <c r="L7" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J7*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>2200</v>
+        <v>3400</v>
       </c>
       <c r="M7" s="11"/>
     </row>
@@ -1206,31 +1197,31 @@
       <c r="B8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="J8" s="5">
         <v>12</v>
       </c>
       <c r="K8" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J8*0.17811)*Data!$F$2), 100)</f>
-        <v>2300</v>
+        <v>3500</v>
       </c>
       <c r="L8" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J8*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>2100</v>
+        <v>3100</v>
       </c>
       <c r="M8" s="11"/>
-      <c r="N8" s="38" t="s">
+      <c r="N8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="41"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="41"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="35"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18"/>
@@ -1238,29 +1229,29 @@
         <v>10</v>
       </c>
       <c r="C9" s="17"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
       <c r="J9" s="6">
         <v>13</v>
       </c>
       <c r="K9" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J9*0.17811)*Data!$F$2), 100)</f>
-        <v>2100</v>
+        <v>3200</v>
       </c>
       <c r="L9" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J9*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1900</v>
+        <v>2900</v>
       </c>
       <c r="M9" s="11"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="41"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="41"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="35"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J10" s="5">
@@ -1268,19 +1259,19 @@
       </c>
       <c r="K10" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J10*0.17811)*Data!$F$2), 100)</f>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="L10" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J10*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1800</v>
+        <v>2700</v>
       </c>
       <c r="M10" s="11"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="41"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="35"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J11" s="6">
@@ -1288,28 +1279,28 @@
       </c>
       <c r="K11" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J11*0.17811)*Data!$F$2), 100)</f>
-        <v>1800</v>
+        <v>2800</v>
       </c>
       <c r="L11" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J11*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1600</v>
+        <v>2500</v>
       </c>
       <c r="M11" s="11"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="41"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="35"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="34"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="33">
         <f>FLOOR(((Data!$G$2*1000)/($B$9*0.17811)*Data!$F$2), 100)</f>
-        <v>2800</v>
+        <v>4200</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
@@ -1319,133 +1310,133 @@
       </c>
       <c r="K12" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J12*0.17811)*Data!$F$2), 100)</f>
-        <v>1700</v>
+        <v>2600</v>
       </c>
       <c r="L12" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J12*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1500</v>
+        <v>2300</v>
       </c>
       <c r="M12" s="11"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="41"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="35"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="34"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="20">
         <f>FLOOR(((Data!$G$2*1000)/($B$9*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>2500</v>
-      </c>
-      <c r="E13" s="37" t="str">
+        <v>3700</v>
+      </c>
+      <c r="E13" s="39" t="str">
         <f>IF(D13&lt;&gt;"", IF(ISNUMBER(SEARCH("LESS", B3)), "⭠Voer deze waarde NIET in bij C=. Deze waarde is puur indicatief. Zie de C waarde naast de tabel.", "⭠Voer de waarde in bij de instelling REG.CAP in het volgende format 00.00T. Bijvoorbeeld 3200L = 03.20T"), "")</f>
         <v>⭠Voer deze waarde NIET in bij C=. Deze waarde is puur indicatief. Zie de C waarde naast de tabel.</v>
       </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
       <c r="J13" s="6">
         <v>17</v>
       </c>
       <c r="K13" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J13*0.17811)*Data!$F$2), 100)</f>
-        <v>1600</v>
+        <v>2400</v>
       </c>
       <c r="L13" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J13*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1400</v>
+        <v>2200</v>
       </c>
       <c r="M13" s="11"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
     </row>
     <row r="14" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
+      <c r="C14" s="44"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
       <c r="J14" s="5">
         <v>18</v>
       </c>
       <c r="K14" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J14*0.17811)*Data!$F$2), 100)</f>
-        <v>1500</v>
+        <v>2300</v>
       </c>
       <c r="L14" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J14*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1400</v>
+        <v>2100</v>
       </c>
       <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
       <c r="J15" s="6">
         <v>19</v>
       </c>
       <c r="K15" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J15*0.17811)*Data!$F$2), 100)</f>
-        <v>1400</v>
+        <v>2200</v>
       </c>
       <c r="L15" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J15*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1300</v>
+        <v>1900</v>
       </c>
       <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
       <c r="J16" s="5">
         <v>20</v>
       </c>
       <c r="K16" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J16*0.17811)*Data!$F$2), 100)</f>
-        <v>1400</v>
+        <v>2100</v>
       </c>
       <c r="L16" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J16*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="M16" s="11"/>
     </row>
     <row r="17" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
       <c r="J17" s="6">
         <v>21</v>
       </c>
       <c r="K17" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J17*0.17811)*Data!$F$2), 100)</f>
-        <v>1300</v>
+        <v>2000</v>
       </c>
       <c r="L17" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J17*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="M17" s="11"/>
     </row>
@@ -1453,38 +1444,38 @@
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
       <c r="J18" s="5">
         <v>22</v>
       </c>
       <c r="K18" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J18*0.17811)*Data!$F$2), 100)</f>
-        <v>1200</v>
+        <v>1900</v>
       </c>
       <c r="L18" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J18*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1100</v>
+        <v>1700</v>
       </c>
       <c r="M18" s="11"/>
     </row>
     <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
       <c r="J19" s="6">
         <v>23</v>
       </c>
       <c r="K19" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J19*0.17811)*Data!$F$2), 100)</f>
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="L19" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J19*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="M19" s="11"/>
     </row>
@@ -1494,11 +1485,11 @@
       </c>
       <c r="K20" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J20*0.17811)*Data!$F$2), 100)</f>
-        <v>1100</v>
+        <v>1700</v>
       </c>
       <c r="L20" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J20*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="M20" s="11"/>
     </row>
@@ -1508,11 +1499,11 @@
       </c>
       <c r="K21" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J21*0.17811)*Data!$F$2), 100)</f>
-        <v>1100</v>
+        <v>1600</v>
       </c>
       <c r="L21" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J21*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="M21" s="11"/>
     </row>
@@ -1522,11 +1513,11 @@
       </c>
       <c r="K22" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J22*0.17811)*Data!$F$2), 100)</f>
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="L22" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J22*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="M22" s="11"/>
     </row>
@@ -1536,11 +1527,11 @@
       </c>
       <c r="K23" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J23*0.17811)*Data!$F$2), 100)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="L23" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J23*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="M23" s="11"/>
     </row>
@@ -1550,11 +1541,11 @@
       </c>
       <c r="K24" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J24*0.17811)*Data!$F$2), 100)</f>
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="L24" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J24*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>900</v>
+        <v>1300</v>
       </c>
       <c r="M24" s="11"/>
     </row>
@@ -1564,11 +1555,11 @@
       </c>
       <c r="K25" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J25*0.17811)*Data!$F$2), 100)</f>
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="L25" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J25*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="M25" s="11"/>
     </row>
@@ -1578,11 +1569,11 @@
       </c>
       <c r="K26" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J26*0.17811)*Data!$F$2), 100)</f>
-        <v>900</v>
+        <v>1400</v>
       </c>
       <c r="L26" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J26*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="M26" s="11"/>
     </row>
@@ -1592,11 +1583,11 @@
       </c>
       <c r="K27" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J27*0.17811)*Data!$F$2), 100)</f>
-        <v>900</v>
+        <v>1300</v>
       </c>
       <c r="L27" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J27*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="M27" s="11"/>
     </row>
@@ -1606,11 +1597,11 @@
       </c>
       <c r="K28" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J28*0.17811)*Data!$F$2), 100)</f>
-        <v>800</v>
+        <v>1300</v>
       </c>
       <c r="L28" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J28*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="M28" s="11"/>
     </row>
@@ -1620,11 +1611,11 @@
       </c>
       <c r="K29" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J29*0.17811)*Data!$F$2), 100)</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="L29" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J29*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="M29" s="11"/>
     </row>
@@ -1634,11 +1625,11 @@
       </c>
       <c r="K30" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J30*0.17811)*Data!$F$2), 100)</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="L30" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J30*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>700</v>
+        <v>1100</v>
       </c>
       <c r="M30" s="11"/>
     </row>
@@ -1648,11 +1639,11 @@
       </c>
       <c r="K31" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J31*0.17811)*Data!$F$2), 100)</f>
-        <v>800</v>
+        <v>1200</v>
       </c>
       <c r="L31" s="14">
         <f>FLOOR(((Data!$G$2*1000)/(J31*0.17811)*Data!$F$2)*0.9, 100)</f>
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="M31" s="11"/>
     </row>
@@ -1725,7 +1716,7 @@
       <c r="C2" s="27"/>
       <c r="F2">
         <f>IF(Dashboard!$B$3="LESS-10",10,IF(Dashboard!$B$3="LESS-15",15,IF(Dashboard!$B$3="LESS-20",20,IF(Dashboard!$B$3="R2D2-32",8,IF(Dashboard!$B$3="R2D2-48",12,IF(Dashboard!$B$3="R2D2-72",18,Dashboard!$B$6))))))</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <f>IF(OR(Dashboard!$B$3="LESS-10",Dashboard!$B$3="LESS-15"),0.499,IF(Dashboard!$B$3="LESS-20",0.62371,0.537))</f>

</xml_diff>